<commit_message>
2022-12-07 Se completa reporte base de budget forecast.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/Reporte_IHS.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/Reporte_IHS.xlsx
@@ -16,14 +16,16 @@
     <sheet name="Aux" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="A_D">Aux!$B$1:$B$2</definedName>
     <definedName name="aplica">Aux!$A$1:$A$2</definedName>
+    <definedName name="YES_NO">Aux!$C$1:$C$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>SI</t>
   </si>
@@ -32,6 +34,15 @@
   </si>
   <si>
     <t>Aplica</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -437,7 +448,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,21 +512,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>